<commit_message>
corections to methods and graph
</commit_message>
<xml_diff>
--- a/2_bootcamp_filter/index-by-cluster.xlsx
+++ b/2_bootcamp_filter/index-by-cluster.xlsx
@@ -442,22 +442,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -467,22 +467,22 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -492,77 +492,77 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
@@ -572,47 +572,47 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -622,27 +622,27 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -652,7 +652,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -662,52 +662,52 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -717,12 +717,12 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -732,37 +732,37 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -772,32 +772,32 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74">
@@ -807,7 +807,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -817,37 +817,37 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84">
@@ -857,42 +857,42 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -902,17 +902,17 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -922,107 +922,107 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -1032,52 +1032,52 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -1087,132 +1087,132 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157">
@@ -1227,32 +1227,32 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165">
@@ -1262,52 +1262,52 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -1317,62 +1317,62 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189">
@@ -1382,32 +1382,32 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -1417,12 +1417,12 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -1432,57 +1432,57 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="211">
@@ -1492,12 +1492,12 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -1507,7 +1507,7 @@
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216">
@@ -1517,7 +1517,7 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -1537,17 +1537,17 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -1567,7 +1567,7 @@
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228">
@@ -1577,7 +1577,7 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -1597,12 +1597,12 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235">
@@ -1612,7 +1612,7 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -1642,22 +1642,22 @@
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="246">
@@ -1677,7 +1677,7 @@
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250">
@@ -1687,17 +1687,17 @@
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
@@ -1712,102 +1712,102 @@
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="276">
@@ -1822,17 +1822,17 @@
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281">
@@ -1842,7 +1842,7 @@
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="283">
@@ -1852,32 +1852,32 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290">
@@ -1887,7 +1887,7 @@
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="292">
@@ -1897,152 +1897,152 @@
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="323">
@@ -2052,27 +2052,27 @@
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="329">
@@ -2082,77 +2082,77 @@
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345">
@@ -2167,27 +2167,27 @@
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="352">
@@ -2197,37 +2197,37 @@
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="360">
@@ -2237,82 +2237,82 @@
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377">
@@ -2322,37 +2322,37 @@
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="385">
@@ -2362,72 +2362,72 @@
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400">

</xml_diff>